<commit_message>
reporting options and Report definitions
</commit_message>
<xml_diff>
--- a/SysSettings.xlsx
+++ b/SysSettings.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VEDA\Veda_models\TIM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF76D145-6C77-451A-8F59-9CDFA2CB17DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C13373ED-2F80-4A7F-8FBB-EA3E02AD1DC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32160" yWindow="2475" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" firstSheet="1" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="28" r:id="rId1"/>
@@ -22,6 +22,7 @@
     <sheet name="Constants" sheetId="25" r:id="rId7"/>
     <sheet name="Defaults" sheetId="26" r:id="rId8"/>
     <sheet name="CPI" sheetId="23" r:id="rId9"/>
+    <sheet name="reporting opt" sheetId="29" r:id="rId10"/>
   </sheets>
   <definedNames>
     <definedName name="__123Graph_AEUMILKPN" localSheetId="0" hidden="1">#REF!</definedName>
@@ -114,7 +115,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="184">
   <si>
     <t>~TFM_UPD</t>
   </si>
@@ -657,6 +658,33 @@
   </si>
   <si>
     <t>James Glynn (UCC, james.glynn@ucc.ie)</t>
+  </si>
+  <si>
+    <t>RPT_OPT</t>
+  </si>
+  <si>
+    <t>ACT~2</t>
+  </si>
+  <si>
+    <t>NCAP~1</t>
+  </si>
+  <si>
+    <t>FLO~3</t>
+  </si>
+  <si>
+    <t>FLO~5</t>
+  </si>
+  <si>
+    <t>FLO~1</t>
+  </si>
+  <si>
+    <t>COMPRD~1</t>
+  </si>
+  <si>
+    <t>OBJ~1</t>
+  </si>
+  <si>
+    <t>ELC~1</t>
   </si>
 </sst>
 </file>
@@ -3906,6 +3934,55 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing9.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>486184</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AD66C175-9474-403C-89BD-BA84D1043970}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4657725" y="266700"/>
+          <a:ext cx="4724809" cy="5924550"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="season_info" displayName="season_info" ref="K4:L16" totalsRowShown="0">
   <tableColumns count="2">
@@ -4260,7 +4337,7 @@
   <sheetPr codeName="Sheet9"/>
   <dimension ref="A1:Z99"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -7101,6 +7178,142 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
   <drawing r:id="rId4"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5B23603-B2D8-4EB8-99EA-37BBDFEDD802}">
+  <dimension ref="C4:E14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P42" sqref="P42"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C6" t="s">
+        <v>175</v>
+      </c>
+      <c r="D6" t="s">
+        <v>176</v>
+      </c>
+      <c r="E6">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="7" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C7" t="s">
+        <v>175</v>
+      </c>
+      <c r="D7" t="s">
+        <v>177</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C8" t="s">
+        <v>175</v>
+      </c>
+      <c r="D8" t="s">
+        <v>178</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C9" t="s">
+        <v>175</v>
+      </c>
+      <c r="D9" t="s">
+        <v>179</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C10" t="s">
+        <v>175</v>
+      </c>
+      <c r="D10" t="s">
+        <v>180</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C11" t="s">
+        <v>175</v>
+      </c>
+      <c r="D11" t="s">
+        <v>181</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C12" t="s">
+        <v>175</v>
+      </c>
+      <c r="D12" t="s">
+        <v>182</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C13" t="s">
+        <v>175</v>
+      </c>
+      <c r="D13" t="s">
+        <v>177</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C14" t="s">
+        <v>175</v>
+      </c>
+      <c r="D14" t="s">
+        <v>183</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>